<commit_message>
major changes: upload data is legacy, processemail is new final endpoint for advanced excel parsing
</commit_message>
<xml_diff>
--- a/TestData/Untitled.xlsx
+++ b/TestData/Untitled.xlsx
@@ -11,9 +11,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>aaaasd@mail.ru</t>
+    </r>
+  </si>
+  <si>
+    <t>test name</t>
   </si>
   <si>
     <r>
@@ -21,35 +33,11 @@
         <b val="1"/>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>aaaasd@mail.ru</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
+        <color indexed="11"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>coolmail@icloud.com</t>
     </r>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>test name</t>
   </si>
   <si>
     <t>test name 2</t>
@@ -88,7 +76,7 @@
       <b val="1"/>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="14"/>
+      <color indexed="11"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -113,12 +101,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="15"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -130,28 +118,6 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -159,28 +125,13 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="13"/>
@@ -189,82 +140,22 @@
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
         <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -274,44 +165,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -331,13 +201,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1369,249 +1238,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="2" width="16.3516" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="B1" t="s" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="5">
-        <v>1</v>
+      <c r="A2" t="s" s="4">
+        <v>2</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" t="s" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="8">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="" tooltip="" display="aaaasd@mail.ru"/>
-    <hyperlink ref="B2" r:id="rId2" location="" tooltip="" display="coolmail@icloud.com"/>
-    <hyperlink ref="E2" r:id="rId3" location="" tooltip="" display="aaaasd@mail.ru"/>
+    <hyperlink ref="A1" r:id="rId1" location="" tooltip="" display="aaaasd@mail.ru"/>
+    <hyperlink ref="A2" r:id="rId2" location="" tooltip="" display="coolmail@icloud.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>